<commit_message>
📊 更新股票資料 2025-11-24 19:52
</commit_message>
<xml_diff>
--- a/StockInfo/otc_analysis_result.xlsx
+++ b/StockInfo/otc_analysis_result.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="20251124" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="20251121" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="20251120" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="20251119" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="20251118" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251124" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251121" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251120" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251119" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251118" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
📊 更新股票資料 2025-11-27 18:01
</commit_message>
<xml_diff>
--- a/StockInfo/otc_analysis_result.xlsx
+++ b/StockInfo/otc_analysis_result.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="20251127" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="20251126" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="20251125" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="20251124" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="20251121" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251127" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251126" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251125" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251124" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251121" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
📊 更新股票資料 2025-12-03 18:30
</commit_message>
<xml_diff>
--- a/StockInfo/otc_analysis_result.xlsx
+++ b/StockInfo/otc_analysis_result.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="20251203" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="20251202" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="20251201" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="20251128" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="20251127" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251203" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251202" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251201" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251128" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251127" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
📊 更新股票資料 2025-12-06 16:38
</commit_message>
<xml_diff>
--- a/StockInfo/otc_analysis_result.xlsx
+++ b/StockInfo/otc_analysis_result.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="20251205" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="20251204" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="20251203" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="20251202" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="20251201" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251205" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251204" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251203" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251202" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251201" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
📊 更新股票資料 2025-12-17 09:40
</commit_message>
<xml_diff>
--- a/StockInfo/otc_analysis_result.xlsx
+++ b/StockInfo/otc_analysis_result.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="20251216" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="20251215" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="20251212" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="20251211" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="20251210" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251216" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251215" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251212" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251211" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251210" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
📊 更新股票資料 2025-12-17 22:05
</commit_message>
<xml_diff>
--- a/StockInfo/otc_analysis_result.xlsx
+++ b/StockInfo/otc_analysis_result.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="20251217" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="20251216" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="20251215" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="20251212" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="20251211" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251217" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251216" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251215" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251212" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251211" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
📊 更新股票資料 2025-12-19 12:24
</commit_message>
<xml_diff>
--- a/StockInfo/otc_analysis_result.xlsx
+++ b/StockInfo/otc_analysis_result.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="20251218" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="20251217" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="20251216" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="20251215" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="20251212" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251218" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251217" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251216" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251215" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251212" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
📊 更新股票資料 2025-12-20 16:40
</commit_message>
<xml_diff>
--- a/StockInfo/otc_analysis_result.xlsx
+++ b/StockInfo/otc_analysis_result.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="20251219" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="20251218" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="20251217" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="20251216" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="20251215" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="彙整分析" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251219" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251218" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251217" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251216" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20251215" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>